<commit_message>
Changes to read excel file
</commit_message>
<xml_diff>
--- a/Data/Input/UiBank Test Data.xlsx
+++ b/Data/Input/UiBank Test Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELLCI5854\Documents\UiPath\UiBank_RPA_Test_Assignment_1\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELLCI5854\Documents\UiPath\UiBank_RPA_Test_Assignment_1_Clone_version\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AED8105-7734-4868-9C4F-C5D23625C736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9FFFFE-83C9-42FC-A53A-35C36D879A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{AB1519B2-5C0E-448B-8AC7-B3DEE8C41096}"/>
   </bookViews>
@@ -1070,17 +1070,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="75f1a19b-876a-4ef4-8ff6-4c7bedccc9b2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94efdb10-7385-4abc-b749-c66a4c8058be">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C33C05F770D5FB42B52C341F090275E6" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="56bfb5869b116298926f6b4e3b7839ac">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94efdb10-7385-4abc-b749-c66a4c8058be" xmlns:ns3="75f1a19b-876a-4ef4-8ff6-4c7bedccc9b2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e8197b2f53f49eb0f5a16722a15e50cf" ns2:_="" ns3:_="">
     <xsd:import namespace="94efdb10-7385-4abc-b749-c66a4c8058be"/>
@@ -1309,6 +1298,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="75f1a19b-876a-4ef4-8ff6-4c7bedccc9b2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94efdb10-7385-4abc-b749-c66a4c8058be">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1319,17 +1319,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1867A13-8479-43A1-9320-63CF239BD3CB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="75f1a19b-876a-4ef4-8ff6-4c7bedccc9b2"/>
-    <ds:schemaRef ds:uri="94efdb10-7385-4abc-b749-c66a4c8058be"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEF74787-EE3B-4B68-95D7-5EDFBDB3739B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1348,6 +1337,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1867A13-8479-43A1-9320-63CF239BD3CB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="75f1a19b-876a-4ef4-8ff6-4c7bedccc9b2"/>
+    <ds:schemaRef ds:uri="94efdb10-7385-4abc-b749-c66a4c8058be"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E7C3CD-E4C7-4AB8-B8BE-D48E3AFED6C0}">
   <ds:schemaRefs>

</xml_diff>